<commit_message>
validation of model 2-1
</commit_message>
<xml_diff>
--- a/results/overview_model_performances.xlsx
+++ b/results/overview_model_performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EigeneDateien\Laura\Studium\Master\3.semester\MaPra\binding_in_disorder\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7651832F-9997-4E13-B8B2-307E06819507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E951CDB-CCD6-4096-AEC0-A2E5C59F2EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Fold</t>
+  </si>
+  <si>
+    <t>simple FNN, residue oversampling</t>
+  </si>
+  <si>
+    <t>"2-1"</t>
   </si>
 </sst>
 </file>
@@ -93,7 +99,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -148,17 +154,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -439,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N17"/>
+  <dimension ref="B2:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +463,7 @@
     <col min="11" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>0</v>
       </c>
@@ -539,7 +550,7 @@
         <v>0.90971299402819739</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -565,27 +576,27 @@
         <v>390</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J6" si="0">F4/(F4+G4)</f>
+        <f t="shared" ref="J4:J8" si="0">F4/(F4+G4)</f>
         <v>0.45907319185794715</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K6" si="1">F4/(F4+I4)</f>
+        <f t="shared" ref="K4:K8" si="1">F4/(F4+I4)</f>
         <v>0.93145869947275928</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L4:L6" si="2">2*((J4*K4)/(J4+K4))</f>
+        <f t="shared" ref="L4:L8" si="2">2*((J4*K4)/(J4+K4))</f>
         <v>0.615027560197273</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ref="M4:M6" si="3">(H4*F4-G4*I4)/SQRT((H4+I4)*(G4+F4)*(H4+G4)*(I4+F4))</f>
+        <f t="shared" ref="M4:M8" si="3">(H4*F4-G4*I4)/SQRT((H4+I4)*(G4+F4)*(H4+G4)*(I4+F4))</f>
         <v>0.59980108664280196</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" ref="N4:N6" si="4">(K4+(H4/(H4+G4)))/2</f>
+        <f t="shared" ref="N4:N8" si="4">(K4+(H4/(H4+G4)))/2</f>
         <v>0.89999389153549969</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -631,7 +642,7 @@
         <v>0.90910174751732775</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -677,43 +688,130 @@
         <v>0.6181040888422259</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="8">
+        <v>53886</v>
+      </c>
+      <c r="G7">
+        <v>5881</v>
+      </c>
+      <c r="H7">
+        <v>39922</v>
+      </c>
+      <c r="I7" s="4">
+        <v>641</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.90160121806347981</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.98824435600711569</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.94293663709381059</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.87272618564319926</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="4"/>
+        <v>0.92992332639995112</v>
+      </c>
+      <c r="R7" s="10"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="8">
+        <v>57604</v>
+      </c>
+      <c r="G8">
+        <v>7009</v>
+      </c>
+      <c r="H8">
+        <v>40492</v>
+      </c>
+      <c r="I8" s="4">
+        <v>60</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.89152337764846079</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.99895948945615987</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.94218863727438518</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.87050989197507322</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="4"/>
+        <v>0.92570235056795691</v>
+      </c>
+      <c r="R8" s="10"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E12" s="4"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N12" s="10"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E16" s="4"/>
       <c r="I16" s="4"/>
     </row>
@@ -723,7 +821,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:I5">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -733,6 +831,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:I6">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:N8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:I7">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -742,13 +860,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:N6">
+  <conditionalFormatting sqref="F8:I8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
validate FNN models with dropout
</commit_message>
<xml_diff>
--- a/results/overview_model_performances.xlsx
+++ b/results/overview_model_performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EigeneDateien\Laura\Studium\Master\3.semester\MaPra\binding_in_disorder\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E951CDB-CCD6-4096-AEC0-A2E5C59F2EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746C91EA-CA50-4993-8590-AECD2AF14580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>"2-1"</t>
+  </si>
+  <si>
+    <t>"2-2"</t>
+  </si>
+  <si>
+    <t>FNN, dropout 0.2</t>
+  </si>
+  <si>
+    <t>FNN, dropout 0.3</t>
   </si>
 </sst>
 </file>
@@ -101,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +129,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -170,6 +185,13 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -453,7 +475,7 @@
   <dimension ref="B2:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,47 +711,47 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="12">
         <v>0.05</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="13">
         <v>53886</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>5881</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>39922</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="14">
         <v>641</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="15">
         <f t="shared" si="0"/>
         <v>0.90160121806347981</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="15">
         <f t="shared" si="1"/>
         <v>0.98824435600711569</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="15">
         <f t="shared" si="2"/>
         <v>0.94293663709381059</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="15">
         <f t="shared" si="3"/>
         <v>0.87272618564319926</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="15">
         <f t="shared" si="4"/>
         <v>0.92992332639995112</v>
       </c>
@@ -783,12 +805,96 @@
       <c r="R8" s="10"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="8">
+        <v>53646</v>
+      </c>
+      <c r="G9">
+        <v>6347</v>
+      </c>
+      <c r="H9">
+        <v>39456</v>
+      </c>
+      <c r="I9" s="4">
+        <v>881</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" ref="J9" si="5">F9/(F9+G9)</f>
+        <v>0.89420432383778103</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" ref="K9" si="6">F9/(F9+I9)</f>
+        <v>0.98384286683661304</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" ref="L9" si="7">2*((J9*K9)/(J9+K9))</f>
+        <v>0.93688438700663634</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" ref="M9" si="8">(H9*F9-G9*I9)/SQRT((H9+I9)*(G9+F9)*(H9+G9)*(I9+F9))</f>
+        <v>0.85871040828181366</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" ref="N9" si="9">(K9+(H9/(H9+G9)))/2</f>
+        <v>0.92263557877996405</v>
+      </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="F10" s="8">
+        <v>57500</v>
+      </c>
+      <c r="G10">
+        <v>6979</v>
+      </c>
+      <c r="H10">
+        <v>40522</v>
+      </c>
+      <c r="I10" s="4">
+        <v>164</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" ref="J10" si="10">F10/(F10+G10)</f>
+        <v>0.89176320972719803</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" ref="K10" si="11">F10/(F10+I10)</f>
+        <v>0.99715593784683687</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" ref="L10" si="12">2*((J10*K10)/(J10+K10))</f>
+        <v>0.9415193666440157</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" ref="M10" si="13">(H10*F10-G10*I10)/SQRT((H10+I10)*(G10+F10)*(H10+G10)*(I10+F10))</f>
+        <v>0.86878022368895469</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" ref="N10" si="14">(K10+(H10/(H10+G10)))/2</f>
+        <v>0.92511635758892019</v>
+      </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E11" s="4"/>
@@ -820,7 +926,38 @@
       <c r="I17" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F3:I5">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:I6">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:N10">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:I7">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -830,7 +967,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:I6">
+  <conditionalFormatting sqref="F8:I8">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -840,27 +977,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:N8">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:I7">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8:I8">
+  <conditionalFormatting sqref="F9:I10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
evaluate model 2-1 on original validation set
</commit_message>
<xml_diff>
--- a/results/overview_model_performances.xlsx
+++ b/results/overview_model_performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EigeneDateien\Laura\Studium\Master\3.semester\MaPra\binding_in_disorder\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746C91EA-CA50-4993-8590-AECD2AF14580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A55D0C-445E-44A8-A9E7-98A37B175B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update model overview, first sketch of multiclass trainer (not tested yet)
</commit_message>
<xml_diff>
--- a/results/overview_model_performances.xlsx
+++ b/results/overview_model_performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EigeneDateien\Laura\Studium\Master\3.semester\MaPra\binding_in_disorder\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A55D0C-445E-44A8-A9E7-98A37B175B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD45CA1-5185-4ABF-8F3D-AEB8C40503DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Model</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>FNN, dropout 0.3</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -165,16 +168,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -192,12 +212,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF23E973"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -472,20 +506,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R17"/>
+  <dimension ref="B2:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.21875" customWidth="1"/>
+    <col min="12" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,23 +546,26 @@
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="2">
+    <row r="3" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="21">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -536,44 +574,48 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.315</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>5240</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>7212</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>38591</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>124</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="18">
+        <f>SUM(F3:I3)</f>
+        <v>51167</v>
+      </c>
+      <c r="K3" s="2">
         <f>F3/(F3+G3)</f>
         <v>0.42081593318342436</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="2">
         <f>F3/(F3+I3)</f>
         <v>0.97688292319164804</v>
       </c>
-      <c r="L3" s="3">
-        <f>2*((J3*K3)/(J3+K3))</f>
+      <c r="M3" s="2">
+        <f>2*((K3*L3)/(K3+L3))</f>
         <v>0.58823529411764708</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="2">
         <f>(H3*F3-G3*I3)/SQRT((H3+I3)*(G3+F3)*(H3+G3)*(I3+F3))</f>
         <v>0.58498117758637802</v>
       </c>
-      <c r="N3" s="3">
-        <f>(K3+(H3/(H3+G3)))/2</f>
+      <c r="O3" s="2">
+        <f>(L3+(H3/(H3+G3)))/2</f>
         <v>0.90971299402819739</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+    <row r="4" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="21">
         <v>1</v>
       </c>
       <c r="C4" t="s">
@@ -582,44 +624,48 @@
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.01</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>5300</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>6245</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>41256</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>390</v>
       </c>
-      <c r="J4" s="3">
-        <f t="shared" ref="J4:J8" si="0">F4/(F4+G4)</f>
+      <c r="J4" s="18">
+        <f t="shared" ref="J4:J11" si="0">SUM(F4:I4)</f>
+        <v>53191</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K8" si="1">F4/(F4+G4)</f>
         <v>0.45907319185794715</v>
       </c>
-      <c r="K4" s="3">
-        <f t="shared" ref="K4:K8" si="1">F4/(F4+I4)</f>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L8" si="2">F4/(F4+I4)</f>
         <v>0.93145869947275928</v>
       </c>
-      <c r="L4" s="3">
-        <f t="shared" ref="L4:L8" si="2">2*((J4*K4)/(J4+K4))</f>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M8" si="3">2*((K4*L4)/(K4+L4))</f>
         <v>0.615027560197273</v>
       </c>
-      <c r="M4" s="3">
-        <f t="shared" ref="M4:M8" si="3">(H4*F4-G4*I4)/SQRT((H4+I4)*(G4+F4)*(H4+G4)*(I4+F4))</f>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N8" si="4">(H4*F4-G4*I4)/SQRT((H4+I4)*(G4+F4)*(H4+G4)*(I4+F4))</f>
         <v>0.59980108664280196</v>
       </c>
-      <c r="N4" s="3">
-        <f t="shared" ref="N4:N8" si="4">(K4+(H4/(H4+G4)))/2</f>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O8" si="5">(L4+(H4/(H4+G4)))/2</f>
         <v>0.89999389153549969</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+    <row r="5" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="21">
         <v>2</v>
       </c>
       <c r="C5" t="s">
@@ -628,44 +674,48 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.06</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>5099</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>6064</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>39739</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>265</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="18">
         <f t="shared" si="0"/>
+        <v>51167</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="1"/>
         <v>0.4567768521006898</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="2">
         <f>F5/(F5+I5)</f>
         <v>0.95059656972408646</v>
       </c>
-      <c r="L5" s="3">
-        <f t="shared" si="2"/>
+      <c r="M5" s="2">
+        <f t="shared" si="3"/>
         <v>0.61705088642826889</v>
       </c>
-      <c r="M5" s="3">
-        <f t="shared" si="3"/>
+      <c r="N5" s="2">
+        <f t="shared" si="4"/>
         <v>0.60689073208504563</v>
       </c>
-      <c r="N5" s="3">
-        <f t="shared" si="4"/>
+      <c r="O5" s="2">
+        <f t="shared" si="5"/>
         <v>0.90910174751732775</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+    <row r="6" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="21">
         <v>3</v>
       </c>
       <c r="C6" t="s">
@@ -674,44 +724,48 @@
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.5</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>4570</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>3929</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>3001</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>1120</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="18">
         <f t="shared" si="0"/>
+        <v>12620</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="1"/>
         <v>0.53771031886104248</v>
       </c>
-      <c r="K6" s="3">
-        <f t="shared" si="1"/>
+      <c r="L6" s="2">
+        <f t="shared" si="2"/>
         <v>0.80316344463971878</v>
       </c>
-      <c r="L6" s="3">
-        <f t="shared" si="2"/>
+      <c r="M6" s="2">
+        <f t="shared" si="3"/>
         <v>0.64416096976531112</v>
       </c>
-      <c r="M6" s="3">
-        <f t="shared" si="3"/>
+      <c r="N6" s="2">
+        <f t="shared" si="4"/>
         <v>0.25062965582900498</v>
       </c>
-      <c r="N6" s="3">
-        <f t="shared" si="4"/>
+      <c r="O6" s="2">
+        <f t="shared" si="5"/>
         <v>0.6181040888422259</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -720,10 +774,10 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>0.05</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>53886</v>
       </c>
       <c r="G7" s="1">
@@ -732,202 +786,284 @@
       <c r="H7" s="1">
         <v>39922</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="13">
         <v>641</v>
       </c>
-      <c r="J7" s="15">
-        <f t="shared" si="0"/>
+      <c r="J7" s="18">
+        <f>SUM(F7:I7)</f>
+        <v>100330</v>
+      </c>
+      <c r="K7" s="14">
+        <f>F7/(F7+G7)</f>
         <v>0.90160121806347981</v>
       </c>
-      <c r="K7" s="15">
-        <f t="shared" si="1"/>
+      <c r="L7" s="14">
+        <f>F7/(F7+I7)</f>
         <v>0.98824435600711569</v>
       </c>
-      <c r="L7" s="15">
-        <f t="shared" si="2"/>
+      <c r="M7" s="14">
+        <f>2*((K7*L7)/(K7+L7))</f>
         <v>0.94293663709381059</v>
       </c>
-      <c r="M7" s="15">
-        <f t="shared" si="3"/>
+      <c r="N7" s="14">
+        <f>(H7*F7-G7*I7)/SQRT((H7+I7)*(G7+F7)*(H7+G7)*(I7+F7))</f>
         <v>0.87272618564319926</v>
       </c>
-      <c r="N7" s="15">
-        <f t="shared" si="4"/>
+      <c r="O7" s="14">
+        <f>(L7+(H7/(H7+G7)))/2</f>
         <v>0.92992332639995112</v>
       </c>
-      <c r="R7" s="10"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5300</v>
+      </c>
+      <c r="G8" s="5">
+        <v>5881</v>
+      </c>
+      <c r="H8" s="16">
+        <v>39922</v>
+      </c>
+      <c r="I8" s="17">
+        <v>64</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" si="0"/>
+        <v>51167</v>
+      </c>
+      <c r="K8" s="2">
+        <f>F8/(F8+G8)</f>
+        <v>0.47401842411233341</v>
+      </c>
+      <c r="L8" s="2">
+        <f>F8/(F8+I8)</f>
+        <v>0.98806860551826992</v>
+      </c>
+      <c r="M8" s="2">
+        <f>2*((K8*L8)/(K8+L8))</f>
+        <v>0.64067694167422184</v>
+      </c>
+      <c r="N8" s="2">
+        <f>(H8*F8-G8*I8)/SQRT((H8+I8)*(G8+F8)*(H8+G8)*(I8+F8))</f>
+        <v>0.6372785037491514</v>
+      </c>
+      <c r="O8" s="2">
+        <f>(L8+(H8/(H8+G8)))/2</f>
+        <v>0.92983545115552824</v>
+      </c>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E9" s="4">
         <v>0.75</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F9" s="7">
         <v>57604</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>7009</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>40492</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I9" s="3">
         <v>60</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J9" s="18">
         <f t="shared" si="0"/>
+        <v>105165</v>
+      </c>
+      <c r="K9" s="2">
+        <f>F9/(F9+G9)</f>
         <v>0.89152337764846079</v>
       </c>
-      <c r="K8" s="3">
-        <f t="shared" si="1"/>
+      <c r="L9" s="2">
+        <f>F9/(F9+I9)</f>
         <v>0.99895948945615987</v>
       </c>
-      <c r="L8" s="3">
-        <f t="shared" si="2"/>
+      <c r="M9" s="2">
+        <f>2*((K9*L9)/(K9+L9))</f>
         <v>0.94218863727438518</v>
       </c>
-      <c r="M8" s="3">
-        <f t="shared" si="3"/>
+      <c r="N9" s="2">
+        <f>(H9*F9-G9*I9)/SQRT((H9+I9)*(G9+F9)*(H9+G9)*(I9+F9))</f>
         <v>0.87050989197507322</v>
       </c>
-      <c r="N8" s="3">
-        <f t="shared" si="4"/>
+      <c r="O9" s="2">
+        <f>(L9+(H9/(H9+G9)))/2</f>
         <v>0.92570235056795691</v>
       </c>
-      <c r="R8" s="10"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="F9" s="8">
-        <v>53646</v>
-      </c>
-      <c r="G9">
-        <v>6347</v>
-      </c>
-      <c r="H9">
-        <v>39456</v>
-      </c>
-      <c r="I9" s="4">
-        <v>881</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" ref="J9" si="5">F9/(F9+G9)</f>
-        <v>0.89420432383778103</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" ref="K9" si="6">F9/(F9+I9)</f>
-        <v>0.98384286683661304</v>
-      </c>
-      <c r="L9" s="3">
-        <f t="shared" ref="L9" si="7">2*((J9*K9)/(J9+K9))</f>
-        <v>0.93688438700663634</v>
-      </c>
-      <c r="M9" s="3">
-        <f t="shared" ref="M9" si="8">(H9*F9-G9*I9)/SQRT((H9+I9)*(G9+F9)*(H9+G9)*(I9+F9))</f>
-        <v>0.85871040828181366</v>
-      </c>
-      <c r="N9" s="3">
-        <f t="shared" ref="N9" si="9">(K9+(H9/(H9+G9)))/2</f>
-        <v>0.92263557877996405</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F10" s="7">
+        <v>53646</v>
+      </c>
+      <c r="G10">
+        <v>6347</v>
+      </c>
+      <c r="H10">
+        <v>39456</v>
+      </c>
+      <c r="I10" s="3">
+        <v>881</v>
+      </c>
+      <c r="J10" s="18">
+        <f t="shared" si="0"/>
+        <v>100330</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" ref="K10" si="6">F10/(F10+G10)</f>
+        <v>0.89420432383778103</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" ref="L10" si="7">F10/(F10+I10)</f>
+        <v>0.98384286683661304</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" ref="M10" si="8">2*((K10*L10)/(K10+L10))</f>
+        <v>0.93688438700663634</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" ref="N10" si="9">(H10*F10-G10*I10)/SQRT((H10+I10)*(G10+F10)*(H10+G10)*(I10+F10))</f>
+        <v>0.85871040828181366</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" ref="O10" si="10">(L10+(H10/(H10+G10)))/2</f>
+        <v>0.92263557877996405</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>4</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E11" s="4">
         <v>0.75</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F11" s="7">
         <v>57500</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>6979</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>40522</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I11" s="3">
         <v>164</v>
       </c>
-      <c r="J10" s="3">
-        <f t="shared" ref="J10" si="10">F10/(F10+G10)</f>
+      <c r="J11" s="18">
+        <f t="shared" si="0"/>
+        <v>105165</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" ref="K11" si="11">F11/(F11+G11)</f>
         <v>0.89176320972719803</v>
       </c>
-      <c r="K10" s="3">
-        <f t="shared" ref="K10" si="11">F10/(F10+I10)</f>
+      <c r="L11" s="2">
+        <f t="shared" ref="L11" si="12">F11/(F11+I11)</f>
         <v>0.99715593784683687</v>
       </c>
-      <c r="L10" s="3">
-        <f t="shared" ref="L10" si="12">2*((J10*K10)/(J10+K10))</f>
+      <c r="M11" s="2">
+        <f t="shared" ref="M11" si="13">2*((K11*L11)/(K11+L11))</f>
         <v>0.9415193666440157</v>
       </c>
-      <c r="M10" s="3">
-        <f t="shared" ref="M10" si="13">(H10*F10-G10*I10)/SQRT((H10+I10)*(G10+F10)*(H10+G10)*(I10+F10))</f>
+      <c r="N11" s="2">
+        <f t="shared" ref="N11" si="14">(H11*F11-G11*I11)/SQRT((H11+I11)*(G11+F11)*(H11+G11)*(I11+F11))</f>
         <v>0.86878022368895469</v>
       </c>
-      <c r="N10" s="3">
-        <f t="shared" ref="N10" si="14">(K10+(H10/(H10+G10)))/2</f>
+      <c r="O11" s="2">
+        <f t="shared" ref="O11" si="15">(L11+(H11/(H11+G11)))/2</f>
         <v>0.92511635758892019</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="N12" s="10"/>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E17" s="4"/>
-      <c r="I17" s="4"/>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="E12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="19"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="E13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="E14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="E15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="E16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="F3:I5">
+  <conditionalFormatting sqref="F3:J3 F8:I8 F4:I5 J4:J11">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:I6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -937,8 +1073,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:I6">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="F7:I7">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -947,17 +1083,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:N10">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:I7">
+  <conditionalFormatting sqref="F9:I9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -967,8 +1093,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:I8">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="F10:I11">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -977,13 +1103,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9:I10">
+  <conditionalFormatting sqref="K3:O11">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
+        <color theme="0"/>
+        <color rgb="FF23E973"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
working version of performance_assessment.py, but still one aspect TODO
</commit_message>
<xml_diff>
--- a/results/overview_model_performances.xlsx
+++ b/results/overview_model_performances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EigeneDateien\Laura\Studium\Master\3.semester\MaPra\binding_in_disorder\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD45CA1-5185-4ABF-8F3D-AEB8C40503DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB600CAB-5B13-4F8E-8EF4-B2EFB4D4020A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4584" yWindow="3552" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Model</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>multilabel, protein-binding</t>
+  </si>
+  <si>
+    <t>multilabel, nuc-binding</t>
+  </si>
+  <si>
+    <t>multilabel, other-binding</t>
+  </si>
+  <si>
+    <t>"4-1"</t>
+  </si>
+  <si>
+    <t>multilabel, class-oversampling, protein-binding</t>
   </si>
 </sst>
 </file>
@@ -151,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -175,15 +190,6 @@
       <right style="thick">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -216,11 +222,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -508,14 +514,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" customWidth="1"/>
     <col min="4" max="4" width="5.21875" customWidth="1"/>
     <col min="12" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -565,7 +571,7 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="21">
+      <c r="B3" s="19">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -615,7 +621,7 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="21">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
       <c r="C4" t="s">
@@ -644,28 +650,28 @@
         <v>53191</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4:K8" si="1">F4/(F4+G4)</f>
+        <f t="shared" ref="K4:K6" si="1">F4/(F4+G4)</f>
         <v>0.45907319185794715</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" ref="L4:L8" si="2">F4/(F4+I4)</f>
+        <f t="shared" ref="L4:L6" si="2">F4/(F4+I4)</f>
         <v>0.93145869947275928</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" ref="M4:M8" si="3">2*((K4*L4)/(K4+L4))</f>
+        <f t="shared" ref="M4:M6" si="3">2*((K4*L4)/(K4+L4))</f>
         <v>0.615027560197273</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" ref="N4:N8" si="4">(H4*F4-G4*I4)/SQRT((H4+I4)*(G4+F4)*(H4+G4)*(I4+F4))</f>
+        <f t="shared" ref="N4:N6" si="4">(H4*F4-G4*I4)/SQRT((H4+I4)*(G4+F4)*(H4+G4)*(I4+F4))</f>
         <v>0.59980108664280196</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" ref="O4:O8" si="5">(L4+(H4/(H4+G4)))/2</f>
+        <f t="shared" ref="O4:O6" si="5">(L4+(H4/(H4+G4)))/2</f>
         <v>0.89999389153549969</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
       <c r="C5" t="s">
@@ -715,7 +721,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="21">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
       <c r="C6" t="s">
@@ -1019,42 +1025,327 @@
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="19"/>
-      <c r="O12" s="9"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="E13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="19"/>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F13" s="20">
+        <v>4121</v>
+      </c>
+      <c r="G13" s="20">
+        <v>5871</v>
+      </c>
+      <c r="H13" s="20">
+        <v>40861</v>
+      </c>
+      <c r="I13" s="3">
+        <v>314</v>
+      </c>
+      <c r="J13" s="18">
+        <f t="shared" ref="J12:J15" si="16">SUM(F13:I13)</f>
+        <v>51167</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" ref="K12:K15" si="17">F13/(F13+G13)</f>
+        <v>0.41242994395516414</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" ref="L12:L15" si="18">F13/(F13+I13)</f>
+        <v>0.92919954904171365</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" ref="M12:M15" si="19">2*((K13*L13)/(K13+L13))</f>
+        <v>0.57128994246898179</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" ref="N12:N15" si="20">(H13*F13-G13*I13)/SQRT((H13+I13)*(G13+F13)*(H13+G13)*(I13+F13))</f>
+        <v>0.57033991947060392</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" ref="O12:O15" si="21">(L13+(H13/(H13+G13)))/2</f>
+        <v>0.90178414497365145</v>
+      </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="E14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="19"/>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F14">
+        <v>492</v>
+      </c>
+      <c r="G14">
+        <v>9556</v>
+      </c>
+      <c r="H14">
+        <v>41068</v>
+      </c>
+      <c r="I14" s="3">
+        <v>51</v>
+      </c>
+      <c r="J14" s="18">
+        <f t="shared" si="16"/>
+        <v>51167</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="17"/>
+        <v>4.8964968152866245E-2</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="18"/>
+        <v>0.90607734806629836</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="19"/>
+        <v>9.2909073741856307E-2</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="20"/>
+        <v>0.18502305007674688</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="21"/>
+        <v>0.85865656278156888</v>
+      </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="E15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="20"/>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="F15">
+        <v>559</v>
+      </c>
+      <c r="G15">
+        <v>9574</v>
+      </c>
+      <c r="H15">
+        <v>41017</v>
+      </c>
+      <c r="I15" s="3">
+        <v>17</v>
+      </c>
+      <c r="J15" s="18">
+        <f t="shared" si="16"/>
+        <v>51167</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="17"/>
+        <v>5.5166288364748843E-2</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="18"/>
+        <v>0.97048611111111116</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="19"/>
+        <v>0.10439816976375013</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="20"/>
+        <v>0.20682024341892377</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="21"/>
+        <v>0.89062148254849904</v>
+      </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="19"/>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="19"/>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="O19" s="9"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F17" s="20">
+        <v>2229</v>
+      </c>
+      <c r="G17" s="20">
+        <v>8200</v>
+      </c>
+      <c r="H17" s="20">
+        <v>37563</v>
+      </c>
+      <c r="I17" s="3">
+        <v>25</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" ref="J16:J19" si="22">SUM(F17:I17)</f>
+        <v>48017</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" ref="K16:K19" si="23">F17/(F17+G17)</f>
+        <v>0.21373094256400421</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" ref="L16:L19" si="24">F17/(F17+I17)</f>
+        <v>0.98890860692102933</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" ref="M16:M19" si="25">2*((K17*L17)/(K17+L17))</f>
+        <v>0.35149412599542695</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" ref="N16:N19" si="26">(H17*F17-G17*I17)/SQRT((H17+I17)*(G17+F17)*(H17+G17)*(I17+F17))</f>
+        <v>0.41536085360907105</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" ref="O16:O19" si="27">(L17+(H17/(H17+G17)))/2</f>
+        <v>0.90486227496587923</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="21">
+        <v>0.45</v>
+      </c>
+      <c r="F18">
+        <v>695</v>
+      </c>
+      <c r="G18">
+        <v>9712</v>
+      </c>
+      <c r="H18">
+        <v>37559</v>
+      </c>
+      <c r="I18" s="3">
+        <v>11</v>
+      </c>
+      <c r="J18" s="18">
+        <f t="shared" si="22"/>
+        <v>47977</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="23"/>
+        <v>6.6781973671567213E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="24"/>
+        <v>0.98441926345609065</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="25"/>
+        <v>0.1250787366147755</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="26"/>
+        <v>0.22758029247420555</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="27"/>
+        <v>0.88948280132462676</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="F19">
+        <v>504</v>
+      </c>
+      <c r="G19">
+        <v>9904</v>
+      </c>
+      <c r="H19">
+        <v>37609</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="22"/>
+        <v>48017</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="23"/>
+        <v>4.8424289008455038E-2</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="25"/>
+        <v>9.2375366568914971E-2</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="26"/>
+        <v>0.19578133833960562</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="27"/>
+        <v>0.89577589291351845</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="F3:J3 F8:I8 F4:I5 J4:J11">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="F3:J3 F8:I8 F4:I5 J4:J19">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1064,6 +1355,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:I6">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:I7">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:I9">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:I11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1073,7 +1394,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:I7">
+  <conditionalFormatting sqref="K3:O19">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J19">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color rgb="FF23E973"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:I13">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1083,7 +1424,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9:I9">
+  <conditionalFormatting sqref="F14:I14">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1093,7 +1434,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:I11">
+  <conditionalFormatting sqref="F15:I15">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17:I17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:I18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1103,23 +1464,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:O11">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="F19:I19">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J11">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color rgb="FF23E973"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>